<commit_message>
Review this. I don't like it?
</commit_message>
<xml_diff>
--- a/Risk Matrix.xlsx
+++ b/Risk Matrix.xlsx
@@ -9,14 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Risk Matrix" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Risk Factors</t>
   </si>
@@ -246,6 +243,18 @@
   </si>
   <si>
     <t>R70</t>
+  </si>
+  <si>
+    <t>Low: 1-2</t>
+  </si>
+  <si>
+    <t>Medium: 2-3</t>
+  </si>
+  <si>
+    <t>High: 3-4</t>
+  </si>
+  <si>
+    <t>IMPACT</t>
   </si>
 </sst>
 </file>
@@ -292,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,8 +323,20 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -367,6 +388,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -375,7 +448,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -387,6 +460,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -513,214 +592,214 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="0">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.41</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.47</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.03</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.54</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.31</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.83</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.26</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.59</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.47</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.99</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.63</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.52</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.18</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.84</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.71</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>3.68</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.72</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.09</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.26</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.68</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.33</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.98</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.56</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.61</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="33">
+                  <c:v>3.76</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.41</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.17</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.48</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.43</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.42</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.86</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.86</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.36</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.03</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.43</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.19</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.55</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.88</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.96</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.93</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.78</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.84</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.47</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.77</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.94</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>3.45</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.76</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.33</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.09</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.03</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.51</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.72</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.04</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.26</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.05</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.24</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.21</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.39</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.84</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.22</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.22</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.99</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.11</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2.23</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2.06</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.47</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.73</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.24</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2.27</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.22</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2.68</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3.06</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3.06</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.12</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>3.57</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3.99</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.02</c:v>
-                </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="67">
+                  <c:v>3.49</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="69">
                   <c:v>3.35</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1.66</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3.97</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3.81</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>2.14</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>2.55</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2.03</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>3.59</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>1.24</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>3.21</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2.07</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>3.69</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>3.81</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>3.37</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>3.83</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>2.64</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>1.35</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>2.76</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>3.07</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>3.83</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>3.44</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>3.55</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>3.67</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>3.57</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>3.66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,11 +1033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2024584704"/>
-        <c:axId val="-2024578560"/>
+        <c:axId val="2110972336"/>
+        <c:axId val="2111359200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2024584704"/>
+        <c:axId val="2110972336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -982,12 +1061,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2024578560"/>
+        <c:crossAx val="2111359200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2024578560"/>
+        <c:axId val="2111359200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,7 +1090,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2024584704"/>
+        <c:crossAx val="2110972336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1669,19 +1748,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Risk Register"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1946,18 +2012,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1971,13 +2038,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <f ca="1">RANDBETWEEN(F2*100,(F2+1)*100)/100</f>
-        <v>3.68</v>
+        <f t="shared" ref="B2:B33" ca="1" si="0">RANDBETWEEN(F2*100,(F2+1)*100)/100</f>
+        <v>3.8</v>
       </c>
       <c r="C2" s="3">
         <v>0.4</v>
@@ -1985,14 +2052,17 @@
       <c r="F2" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L2" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <f ca="1">RANDBETWEEN(F3*100,(F3+1)*100)/100</f>
-        <v>3.72</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.16</v>
       </c>
       <c r="C3" s="4">
         <v>0.1</v>
@@ -2000,14 +2070,17 @@
       <c r="F3" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L3" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <f ca="1">RANDBETWEEN(F4*100,(F4+1)*100)/100</f>
-        <v>2.09</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.39</v>
       </c>
       <c r="C4" s="5">
         <v>0.9</v>
@@ -2015,14 +2088,17 @@
       <c r="F4" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L4" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <f ca="1">RANDBETWEEN(F5*100,(F5+1)*100)/100</f>
-        <v>3.75</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.41</v>
       </c>
       <c r="C5" s="3">
         <v>0.65</v>
@@ -2030,14 +2106,17 @@
       <c r="F5" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="L5" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <f ca="1">RANDBETWEEN(F6*100,(F6+1)*100)/100</f>
-        <v>3.26</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.25</v>
       </c>
       <c r="C6" s="4">
         <v>0.15</v>
@@ -2046,13 +2125,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2">
-        <f ca="1">RANDBETWEEN(F7*100,(F7+1)*100)/100</f>
-        <v>2.68</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.84</v>
       </c>
       <c r="C7" s="4">
         <v>0.05</v>
@@ -2061,13 +2140,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2">
-        <f ca="1">RANDBETWEEN(F8*100,(F8+1)*100)/100</f>
-        <v>3.33</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.47</v>
       </c>
       <c r="C8" s="4">
         <v>0.05</v>
@@ -2076,13 +2155,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <f ca="1">RANDBETWEEN(F9*100,(F9+1)*100)/100</f>
-        <v>3.98</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.54</v>
       </c>
       <c r="C9" s="3">
         <v>0.4</v>
@@ -2091,13 +2170,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2">
-        <f ca="1">RANDBETWEEN(F10*100,(F10+1)*100)/100</f>
-        <v>3.56</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.38</v>
       </c>
       <c r="C10" s="4">
         <v>0.2</v>
@@ -2106,13 +2185,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2">
-        <f ca="1">RANDBETWEEN(F11*100,(F11+1)*100)/100</f>
-        <v>2.2999999999999998</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0299999999999998</v>
       </c>
       <c r="C11" s="4">
         <v>0.1</v>
@@ -2121,13 +2200,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2">
-        <f ca="1">RANDBETWEEN(F12*100,(F12+1)*100)/100</f>
-        <v>2.61</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5499999999999998</v>
       </c>
       <c r="C12" s="4">
         <v>0.12</v>
@@ -2136,13 +2215,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2">
-        <f ca="1">RANDBETWEEN(F13*100,(F13+1)*100)/100</f>
-        <v>3.45</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.54</v>
       </c>
       <c r="C13" s="5">
         <v>0.75</v>
@@ -2151,13 +2230,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2">
-        <f ca="1">RANDBETWEEN(F14*100,(F14+1)*100)/100</f>
-        <v>2.76</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.31</v>
       </c>
       <c r="C14" s="4">
         <v>0.15</v>
@@ -2166,13 +2245,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="2">
-        <f ca="1">RANDBETWEEN(F15*100,(F15+1)*100)/100</f>
-        <v>3.33</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.83</v>
       </c>
       <c r="C15" s="3">
         <v>0.35</v>
@@ -2181,13 +2260,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="2">
-        <f ca="1">RANDBETWEEN(F16*100,(F16+1)*100)/100</f>
-        <v>3.09</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.26</v>
       </c>
       <c r="C16" s="4">
         <v>0.15</v>
@@ -2201,8 +2280,8 @@
         <v>18</v>
       </c>
       <c r="B17" s="2">
-        <f ca="1">RANDBETWEEN(F17*100,(F17+1)*100)/100</f>
-        <v>3.8</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.59</v>
       </c>
       <c r="C17" s="4">
         <v>0.05</v>
@@ -2216,8 +2295,8 @@
         <v>19</v>
       </c>
       <c r="B18" s="2">
-        <f ca="1">RANDBETWEEN(F18*100,(F18+1)*100)/100</f>
-        <v>1.03</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.73</v>
       </c>
       <c r="C18" s="5">
         <v>0.75</v>
@@ -2231,8 +2310,8 @@
         <v>20</v>
       </c>
       <c r="B19" s="2">
-        <f ca="1">RANDBETWEEN(F19*100,(F19+1)*100)/100</f>
-        <v>3.51</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.47</v>
       </c>
       <c r="C19" s="4">
         <v>0.15</v>
@@ -2246,8 +2325,8 @@
         <v>21</v>
       </c>
       <c r="B20" s="2">
-        <f ca="1">RANDBETWEEN(F20*100,(F20+1)*100)/100</f>
-        <v>1.72</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4</v>
       </c>
       <c r="C20" s="4">
         <v>0.3</v>
@@ -2261,8 +2340,8 @@
         <v>22</v>
       </c>
       <c r="B21" s="2">
-        <f ca="1">RANDBETWEEN(F21*100,(F21+1)*100)/100</f>
-        <v>2.04</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.99</v>
       </c>
       <c r="C21" s="4">
         <v>0.15</v>
@@ -2276,8 +2355,8 @@
         <v>23</v>
       </c>
       <c r="B22" s="2">
-        <f ca="1">RANDBETWEEN(F22*100,(F22+1)*100)/100</f>
-        <v>3.26</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.2</v>
       </c>
       <c r="C22" s="4">
         <v>0.4</v>
@@ -2291,8 +2370,8 @@
         <v>24</v>
       </c>
       <c r="B23" s="2">
-        <f ca="1">RANDBETWEEN(F23*100,(F23+1)*100)/100</f>
-        <v>3.05</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.88</v>
       </c>
       <c r="C23" s="4">
         <v>0.15</v>
@@ -2306,8 +2385,8 @@
         <v>25</v>
       </c>
       <c r="B24" s="2">
-        <f ca="1">RANDBETWEEN(F24*100,(F24+1)*100)/100</f>
-        <v>3.24</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.63</v>
       </c>
       <c r="C24" s="3">
         <v>0.6</v>
@@ -2321,8 +2400,8 @@
         <v>26</v>
       </c>
       <c r="B25" s="2">
-        <f ca="1">RANDBETWEEN(F25*100,(F25+1)*100)/100</f>
-        <v>2.21</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="C25" s="3">
         <v>0.35</v>
@@ -2336,8 +2415,8 @@
         <v>27</v>
       </c>
       <c r="B26" s="2">
-        <f ca="1">RANDBETWEEN(F26*100,(F26+1)*100)/100</f>
-        <v>3.39</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.52</v>
       </c>
       <c r="C26" s="4">
         <v>0.03</v>
@@ -2351,8 +2430,8 @@
         <v>28</v>
       </c>
       <c r="B27" s="2">
-        <f ca="1">RANDBETWEEN(F27*100,(F27+1)*100)/100</f>
-        <v>3.84</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.18</v>
       </c>
       <c r="C27" s="3">
         <v>0.55000000000000004</v>
@@ -2366,8 +2445,8 @@
         <v>29</v>
       </c>
       <c r="B28" s="2">
-        <f ca="1">RANDBETWEEN(F28*100,(F28+1)*100)/100</f>
-        <v>2.2200000000000002</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.17</v>
       </c>
       <c r="C28" s="4">
         <v>0.2</v>
@@ -2381,8 +2460,8 @@
         <v>30</v>
       </c>
       <c r="B29" s="2">
-        <f ca="1">RANDBETWEEN(F29*100,(F29+1)*100)/100</f>
-        <v>3.22</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.75</v>
       </c>
       <c r="C29" s="4">
         <v>0.15</v>
@@ -2396,8 +2475,8 @@
         <v>31</v>
       </c>
       <c r="B30" s="2">
-        <f ca="1">RANDBETWEEN(F30*100,(F30+1)*100)/100</f>
-        <v>2.99</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.98</v>
       </c>
       <c r="C30" s="4">
         <v>0.15</v>
@@ -2411,8 +2490,8 @@
         <v>32</v>
       </c>
       <c r="B31" s="2">
-        <f ca="1">RANDBETWEEN(F31*100,(F31+1)*100)/100</f>
-        <v>2.11</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.77</v>
       </c>
       <c r="C31" s="4">
         <v>0.1</v>
@@ -2426,8 +2505,8 @@
         <v>33</v>
       </c>
       <c r="B32" s="2">
-        <f ca="1">RANDBETWEEN(F32*100,(F32+1)*100)/100</f>
-        <v>2.23</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.84</v>
       </c>
       <c r="C32" s="4">
         <v>0.1</v>
@@ -2441,8 +2520,8 @@
         <v>34</v>
       </c>
       <c r="B33" s="2">
-        <f ca="1">RANDBETWEEN(F33*100,(F33+1)*100)/100</f>
-        <v>2.06</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.71</v>
       </c>
       <c r="C33" s="4">
         <v>7.0000000000000007E-2</v>
@@ -2456,8 +2535,8 @@
         <v>35</v>
       </c>
       <c r="B34" s="2">
-        <f ca="1">RANDBETWEEN(F34*100,(F34+1)*100)/100</f>
-        <v>3.47</v>
+        <f t="shared" ref="B34:B65" ca="1" si="1">RANDBETWEEN(F34*100,(F34+1)*100)/100</f>
+        <v>3.68</v>
       </c>
       <c r="C34" s="4">
         <v>0.02</v>
@@ -2471,8 +2550,8 @@
         <v>36</v>
       </c>
       <c r="B35" s="2">
-        <f ca="1">RANDBETWEEN(F35*100,(F35+1)*100)/100</f>
-        <v>3.73</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.76</v>
       </c>
       <c r="C35" s="4">
         <v>0.02</v>
@@ -2486,8 +2565,8 @@
         <v>37</v>
       </c>
       <c r="B36" s="2">
-        <f ca="1">RANDBETWEEN(F36*100,(F36+1)*100)/100</f>
-        <v>1.24</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.83</v>
       </c>
       <c r="C36" s="4">
         <v>0.23</v>
@@ -2501,8 +2580,8 @@
         <v>38</v>
       </c>
       <c r="B37" s="2">
-        <f ca="1">RANDBETWEEN(F37*100,(F37+1)*100)/100</f>
-        <v>2.27</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.41</v>
       </c>
       <c r="C37" s="4">
         <v>0.17</v>
@@ -2516,8 +2595,8 @@
         <v>39</v>
       </c>
       <c r="B38" s="2">
-        <f ca="1">RANDBETWEEN(F38*100,(F38+1)*100)/100</f>
-        <v>3.22</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.17</v>
       </c>
       <c r="C38" s="4">
         <v>0.1</v>
@@ -2531,8 +2610,8 @@
         <v>40</v>
       </c>
       <c r="B39" s="2">
-        <f ca="1">RANDBETWEEN(F39*100,(F39+1)*100)/100</f>
-        <v>2.68</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.65</v>
       </c>
       <c r="C39" s="3">
         <v>0.6</v>
@@ -2546,8 +2625,8 @@
         <v>41</v>
       </c>
       <c r="B40" s="2">
-        <f ca="1">RANDBETWEEN(F40*100,(F40+1)*100)/100</f>
-        <v>3.06</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.15</v>
       </c>
       <c r="C40" s="4">
         <v>0.05</v>
@@ -2561,8 +2640,8 @@
         <v>42</v>
       </c>
       <c r="B41" s="2">
-        <f ca="1">RANDBETWEEN(F41*100,(F41+1)*100)/100</f>
-        <v>3.06</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.42</v>
       </c>
       <c r="C41" s="4">
         <v>0.03</v>
@@ -2576,8 +2655,8 @@
         <v>43</v>
       </c>
       <c r="B42" s="2">
-        <f ca="1">RANDBETWEEN(F42*100,(F42+1)*100)/100</f>
-        <v>3.12</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.48</v>
       </c>
       <c r="C42" s="4">
         <v>0.03</v>
@@ -2591,8 +2670,8 @@
         <v>44</v>
       </c>
       <c r="B43" s="2">
-        <f ca="1">RANDBETWEEN(F43*100,(F43+1)*100)/100</f>
-        <v>3.57</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.43</v>
       </c>
       <c r="C43" s="4">
         <v>0.08</v>
@@ -2606,8 +2685,8 @@
         <v>45</v>
       </c>
       <c r="B44" s="2">
-        <f ca="1">RANDBETWEEN(F44*100,(F44+1)*100)/100</f>
-        <v>3.99</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.53</v>
       </c>
       <c r="C44" s="4">
         <v>0.05</v>
@@ -2621,8 +2700,8 @@
         <v>46</v>
       </c>
       <c r="B45" s="2">
-        <f ca="1">RANDBETWEEN(F45*100,(F45+1)*100)/100</f>
-        <v>1.02</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.42</v>
       </c>
       <c r="C45" s="3">
         <v>0.6</v>
@@ -2636,8 +2715,8 @@
         <v>47</v>
       </c>
       <c r="B46" s="2">
-        <f ca="1">RANDBETWEEN(F46*100,(F46+1)*100)/100</f>
-        <v>3.35</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.86</v>
       </c>
       <c r="C46" s="4">
         <v>0.12</v>
@@ -2651,8 +2730,8 @@
         <v>48</v>
       </c>
       <c r="B47" s="2">
-        <f ca="1">RANDBETWEEN(F47*100,(F47+1)*100)/100</f>
-        <v>1.66</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.86</v>
       </c>
       <c r="C47" s="4">
         <v>7.0000000000000007E-2</v>
@@ -2666,8 +2745,8 @@
         <v>49</v>
       </c>
       <c r="B48" s="2">
-        <f ca="1">RANDBETWEEN(F48*100,(F48+1)*100)/100</f>
-        <v>3.97</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.36</v>
       </c>
       <c r="C48" s="4">
         <v>0.17</v>
@@ -2681,8 +2760,8 @@
         <v>50</v>
       </c>
       <c r="B49" s="2">
-        <f ca="1">RANDBETWEEN(F49*100,(F49+1)*100)/100</f>
-        <v>3.81</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.39</v>
       </c>
       <c r="C49" s="4">
         <v>0.08</v>
@@ -2696,8 +2775,8 @@
         <v>51</v>
       </c>
       <c r="B50" s="2">
-        <f ca="1">RANDBETWEEN(F50*100,(F50+1)*100)/100</f>
-        <v>2.14</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.0299999999999998</v>
       </c>
       <c r="C50" s="4">
         <v>0.1</v>
@@ -2711,8 +2790,8 @@
         <v>52</v>
       </c>
       <c r="B51" s="2">
-        <f ca="1">RANDBETWEEN(F51*100,(F51+1)*100)/100</f>
-        <v>2.5499999999999998</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="C51" s="3">
         <v>0.4</v>
@@ -2726,8 +2805,8 @@
         <v>53</v>
       </c>
       <c r="B52" s="2">
-        <f ca="1">RANDBETWEEN(F52*100,(F52+1)*100)/100</f>
-        <v>2.0299999999999998</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.19</v>
       </c>
       <c r="C52" s="5">
         <v>0.85</v>
@@ -2741,8 +2820,8 @@
         <v>54</v>
       </c>
       <c r="B53" s="2">
-        <f ca="1">RANDBETWEEN(F53*100,(F53+1)*100)/100</f>
-        <v>3.59</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.55</v>
       </c>
       <c r="C53" s="3">
         <v>0.5</v>
@@ -2756,8 +2835,8 @@
         <v>55</v>
       </c>
       <c r="B54" s="2">
-        <f ca="1">RANDBETWEEN(F54*100,(F54+1)*100)/100</f>
-        <v>1.24</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.88</v>
       </c>
       <c r="C54" s="3">
         <v>0.5</v>
@@ -2771,8 +2850,8 @@
         <v>56</v>
       </c>
       <c r="B55" s="2">
-        <f ca="1">RANDBETWEEN(F55*100,(F55+1)*100)/100</f>
-        <v>2.75</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.48</v>
       </c>
       <c r="C55" s="4">
         <v>0.1</v>
@@ -2786,8 +2865,8 @@
         <v>57</v>
       </c>
       <c r="B56" s="2">
-        <f ca="1">RANDBETWEEN(F56*100,(F56+1)*100)/100</f>
-        <v>3.21</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.39</v>
       </c>
       <c r="C56" s="4">
         <v>0.03</v>
@@ -2801,8 +2880,8 @@
         <v>58</v>
       </c>
       <c r="B57" s="2">
-        <f ca="1">RANDBETWEEN(F57*100,(F57+1)*100)/100</f>
-        <v>2.0699999999999998</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.64</v>
       </c>
       <c r="C57" s="4">
         <v>7.4999999999999997E-2</v>
@@ -2816,8 +2895,8 @@
         <v>59</v>
       </c>
       <c r="B58" s="2">
-        <f ca="1">RANDBETWEEN(F58*100,(F58+1)*100)/100</f>
-        <v>3.69</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.96</v>
       </c>
       <c r="C58" s="4">
         <v>0.03</v>
@@ -2831,8 +2910,8 @@
         <v>60</v>
       </c>
       <c r="B59" s="2">
-        <f ca="1">RANDBETWEEN(F59*100,(F59+1)*100)/100</f>
-        <v>3.81</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.93</v>
       </c>
       <c r="C59" s="4">
         <v>0.02</v>
@@ -2846,8 +2925,8 @@
         <v>61</v>
       </c>
       <c r="B60" s="2">
-        <f ca="1">RANDBETWEEN(F60*100,(F60+1)*100)/100</f>
-        <v>3.37</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.78</v>
       </c>
       <c r="C60" s="4">
         <v>0.12</v>
@@ -2861,8 +2940,8 @@
         <v>62</v>
       </c>
       <c r="B61" s="2">
-        <f ca="1">RANDBETWEEN(F61*100,(F61+1)*100)/100</f>
-        <v>3.83</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.03</v>
       </c>
       <c r="C61" s="3">
         <v>0.45</v>
@@ -2876,8 +2955,8 @@
         <v>63</v>
       </c>
       <c r="B62" s="2">
-        <f ca="1">RANDBETWEEN(F62*100,(F62+1)*100)/100</f>
-        <v>2.64</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.84</v>
       </c>
       <c r="C62" s="5">
         <v>0.7</v>
@@ -2891,8 +2970,8 @@
         <v>64</v>
       </c>
       <c r="B63" s="2">
-        <f ca="1">RANDBETWEEN(F63*100,(F63+1)*100)/100</f>
-        <v>1.35</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.33</v>
       </c>
       <c r="C63" s="4">
         <v>0.25</v>
@@ -2906,8 +2985,8 @@
         <v>65</v>
       </c>
       <c r="B64" s="2">
-        <f ca="1">RANDBETWEEN(F64*100,(F64+1)*100)/100</f>
-        <v>2.76</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.38</v>
       </c>
       <c r="C64" s="5">
         <v>1</v>
@@ -2921,8 +3000,8 @@
         <v>66</v>
       </c>
       <c r="B65" s="2">
-        <f ca="1">RANDBETWEEN(F65*100,(F65+1)*100)/100</f>
-        <v>3.07</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.47</v>
       </c>
       <c r="C65" s="4">
         <v>0.04</v>
@@ -2936,8 +3015,8 @@
         <v>67</v>
       </c>
       <c r="B66" s="2">
-        <f ca="1">RANDBETWEEN(F66*100,(F66+1)*100)/100</f>
-        <v>3.83</v>
+        <f t="shared" ref="B66:B71" ca="1" si="2">RANDBETWEEN(F66*100,(F66+1)*100)/100</f>
+        <v>3.77</v>
       </c>
       <c r="C66" s="4">
         <v>0.23</v>
@@ -2951,8 +3030,8 @@
         <v>68</v>
       </c>
       <c r="B67" s="2">
-        <f ca="1">RANDBETWEEN(F67*100,(F67+1)*100)/100</f>
-        <v>3.44</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.94</v>
       </c>
       <c r="C67" s="3">
         <v>0.65</v>
@@ -2966,8 +3045,8 @@
         <v>69</v>
       </c>
       <c r="B68" s="2">
-        <f ca="1">RANDBETWEEN(F68*100,(F68+1)*100)/100</f>
-        <v>3.55</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.45</v>
       </c>
       <c r="C68" s="3">
         <v>0.65</v>
@@ -2981,8 +3060,8 @@
         <v>70</v>
       </c>
       <c r="B69" s="2">
-        <f ca="1">RANDBETWEEN(F69*100,(F69+1)*100)/100</f>
-        <v>3.67</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.49</v>
       </c>
       <c r="C69" s="4">
         <v>0.05</v>
@@ -2996,8 +3075,8 @@
         <v>71</v>
       </c>
       <c r="B70" s="2">
-        <f ca="1">RANDBETWEEN(F70*100,(F70+1)*100)/100</f>
-        <v>3.57</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.88</v>
       </c>
       <c r="C70" s="4">
         <v>0.01</v>
@@ -3011,8 +3090,8 @@
         <v>72</v>
       </c>
       <c r="B71" s="2">
-        <f ca="1">RANDBETWEEN(F71*100,(F71+1)*100)/100</f>
-        <v>3.66</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.35</v>
       </c>
       <c r="C71" s="9">
         <v>0.01</v>

</xml_diff>